<commit_message>
JSON Schema validation from excel input
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -10,12 +10,11 @@
     <sheet name="testData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>dataKey</t>
   </si>
@@ -73,18 +72,115 @@
   </si>
   <si>
     <t>addBookDetail</t>
+  </si>
+  <si>
+    <t>responseSchema</t>
+  </si>
+  <si>
+    <t>{
+      "title": "Game of Throne",
+      "body": "Here will be description of the Book",
+      "userId": "911",
+      "id": 1213
+}</t>
+  </si>
+  <si>
+    <t>{
+  "definitions": {},
+  "$schema": "http://json-schema.org/draft-07/schema#",
+  "$id": "http://example.com/root.json",
+  "type": "object",
+  "required": [
+    "title",
+    "body",
+    "userId",
+    "id"
+  ],
+  "properties": {
+    "title": {
+      "$id": "#/properties/title",
+      "type": "string"
+    },
+    "body": {
+      "$id": "#/properties/body",
+      "type": "string"
+    },
+    "userId": {
+      "$id": "#/properties/userId",
+      "type": "string"
+    },
+    "id": {
+      "$id": "#/properties/id",
+      "type": "integer"
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "name": "Tester",
+    "job": "Automation",
+    "id": "128",
+    "createdAt": "2019-03-22T18:58:35.153Z"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "definitions": {},
+  "$schema": "http://json-schema.org/draft-07/schema#",
+  "$id": "http://example.com/root.json",
+  "type": "object",
+  "required": [
+    "name",
+    "job",
+    "id",
+    "createdAt"
+  ],
+  "properties": {
+    "name": {
+      "$id": "#/properties/name",
+      "type": "string"
+    },
+    "job": {
+      "$id": "#/properties/job",
+      "type": "string"
+    },
+    "id": {
+      "$id": "#/properties/id",
+      "type": "string"
+    },
+    "createdAt": {
+      "$id": "#/properties/createdAt",
+      "type": "string"
+    }
+  }
+}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -116,21 +212,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -401,22 +500,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.85546875" style="1"/>
+    <col min="1" max="1" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,46 +527,60 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="90">
+    <row r="2" spans="1:5" ht="90">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="90">
+    <row r="3" spans="1:5" ht="90">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60">
+    <row r="4" spans="1:5" ht="90">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
+    <row r="5" spans="1:5">
+      <c r="B5" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -477,5 +589,6 @@
     <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Extent report and logs
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Space\workspace\API-Cucumber\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBCDEC2-7B6D-44C9-AB2A-FCA85E8EF444}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1096D74D-E3EC-43D6-AD57-F97AB6017EB0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -760,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1"/>

</xml_diff>